<commit_message>
commit latest query count file
</commit_message>
<xml_diff>
--- a/Outputs/DQ Report Query count.xlsx
+++ b/Outputs/DQ Report Query count.xlsx
@@ -53,49 +53,49 @@
     <t xml:space="preserve">03. HZ Two or more dose 2</t>
   </si>
   <si>
+    <t xml:space="preserve">06. COV Booster interval &lt; 12 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. COV Dose 2, no dose 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. COV Dose 1 and booster, no dose 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. FLU interval &lt; 4 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16. HZ Dose 2 interval &lt; 56 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. HZ Shingrix dose 2, Zostavax dose 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18. HZ Dose 2, no dose 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20. HZ Vacc given outwith age guidance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21. PNEUM Vacc interval &lt; 260 weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22. PNEUM Vacc given outwith age guidance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24. RSV Non-cohort vacc age&gt;55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25. COV Two or more boosters in campaign</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26. COV Outwith vacc programme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27. COV Vacc given outwith age guidance</t>
+  </si>
+  <si>
     <t xml:space="preserve">04. COV Two or more dose 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. COV Dose 2, no dose 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11. COV Dose 1 and booster, no dose 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12. FLU interval &lt; 4 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16. HZ Dose 2 interval &lt; 56 days</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17. HZ Shingrix dose 2, Zostavax dose 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18. HZ Dose 2, no dose 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20. HZ Vacc given outwith age guidance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21. PNEUM Vacc interval &lt; 260 weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22. PNEUM Vacc given outwith age guidance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24. RSV Non-cohort vacc age&gt;55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25. COV Two or more boosters in campaign</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26. COV Outwith vacc programme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27. COV Vacc given outwith age guidance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06. COV Booster interval &lt; 12 weeks</t>
   </si>
   <si>
     <t xml:space="preserve">14. FLU LAIV given age &lt;2 or &gt;18</t>
@@ -519,19 +519,19 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E2" t="n">
         <v>4</v>
       </c>
       <c r="F2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
@@ -539,19 +539,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C3" t="n">
+        <v>53</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E3" t="n">
         <v>45</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E3" t="n">
-        <v>40</v>
-      </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -559,33 +559,39 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E4" t="n">
         <v>6</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4"/>
-      <c r="F4"/>
+      <c r="F4" t="n">
+        <v>-2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C5" t="n">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E5" t="n">
         <v>35</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E5" t="n">
-        <v>49</v>
-      </c>
       <c r="F5" t="n">
-        <v>-14</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="6">
@@ -593,16 +599,16 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C6" t="n">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E6" t="n">
         <v>30</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E6" t="n">
-        <v>22</v>
       </c>
       <c r="F6" t="n">
         <v>8</v>
@@ -613,19 +619,19 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C7" t="n">
+        <v>42</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E7" t="n">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E7" t="n">
-        <v>28</v>
-      </c>
       <c r="F7" t="n">
-        <v>16</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="8">
@@ -633,19 +639,19 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C8" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -653,39 +659,33 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C9" t="n">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
+      <c r="D9" s="1"/>
+      <c r="E9"/>
+      <c r="F9"/>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E10" t="n">
         <v>6</v>
       </c>
-      <c r="D10" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E10" t="n">
-        <v>7</v>
-      </c>
       <c r="F10" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="11">
@@ -693,13 +693,13 @@
         <v>15</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C11" t="n">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E11" t="n">
         <v>6</v>
@@ -713,33 +713,39 @@
         <v>16</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E12" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12"/>
-      <c r="F12"/>
+      <c r="F12" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C13" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E13" t="n">
         <v>5</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4</v>
-      </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -747,19 +753,19 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C14" t="n">
         <v>3</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E14" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F14" t="n">
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -767,19 +773,19 @@
         <v>19</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C15" t="n">
         <v>16</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E15" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F15" t="n">
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -787,19 +793,19 @@
         <v>20</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C16" t="n">
+        <v>429</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E16" t="n">
         <v>493</v>
       </c>
-      <c r="D16" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E16" t="n">
-        <v>556</v>
-      </c>
       <c r="F16" t="n">
-        <v>-63</v>
+        <v>-64</v>
       </c>
     </row>
     <row r="17">
@@ -807,19 +813,19 @@
         <v>21</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C17" t="n">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E17" t="n">
         <v>21</v>
       </c>
-      <c r="D17" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E17" t="n">
-        <v>25</v>
-      </c>
       <c r="F17" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="18">
@@ -827,19 +833,19 @@
         <v>22</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C18" t="n">
+        <v>462</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E18" t="n">
         <v>445</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E18" t="n">
-        <v>497</v>
-      </c>
       <c r="F18" t="n">
-        <v>-52</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19">
@@ -847,19 +853,19 @@
         <v>23</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C19" t="n">
+        <v>79</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E19" t="n">
         <v>65</v>
       </c>
-      <c r="D19" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E19" t="n">
-        <v>64</v>
-      </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
@@ -867,33 +873,39 @@
         <v>24</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E20" t="n">
         <v>4</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20"/>
-      <c r="F20"/>
+      <c r="F20" t="n">
+        <v>-2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C21" t="n">
+        <v>141</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E21" t="n">
         <v>179</v>
       </c>
-      <c r="D21" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E21" t="n">
-        <v>198</v>
-      </c>
       <c r="F21" t="n">
-        <v>-19</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="22">
@@ -901,19 +913,19 @@
         <v>26</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>45888</v>
+        <v>45895</v>
       </c>
       <c r="C22" t="n">
+        <v>137</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <v>45888</v>
+      </c>
+      <c r="E22" t="n">
         <v>173</v>
       </c>
-      <c r="D22" s="1" t="n">
-        <v>45881</v>
-      </c>
-      <c r="E22" t="n">
-        <v>181</v>
-      </c>
       <c r="F22" t="n">
-        <v>-8</v>
+        <v>-36</v>
       </c>
     </row>
     <row r="23">
@@ -923,7 +935,7 @@
       <c r="B23" s="1"/>
       <c r="C23"/>
       <c r="D23" s="1" t="n">
-        <v>45881</v>
+        <v>45888</v>
       </c>
       <c r="E23" t="n">
         <v>2</v>

</xml_diff>